<commit_message>
Chép xong tất các code từ file pdf ra và chạy
</commit_message>
<xml_diff>
--- a/user_data.xlsx
+++ b/user_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taqua\My-Repo\HK9\He-thong-thong-tin-thong-minh-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF82AF8-6824-4A55-9FD2-C73D50312556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18DF424-F0E7-4EB1-AE7E-175186F4F0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -351,267 +351,265 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="C1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
+    <row r="1" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C2">
         <v>19</v>
       </c>
-      <c r="B2">
+      <c r="D2">
         <v>19000</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C3">
         <v>35</v>
       </c>
-      <c r="B3">
+      <c r="D3">
         <v>20000</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C4">
         <v>26</v>
       </c>
-      <c r="B4">
+      <c r="D4">
         <v>43000</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C5">
         <v>27</v>
       </c>
-      <c r="B5">
+      <c r="D5">
         <v>57000</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C6">
         <v>19</v>
       </c>
-      <c r="B6">
+      <c r="D6">
         <v>76000</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C7">
         <v>27</v>
       </c>
-      <c r="B7">
+      <c r="D7">
         <v>58000</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C8">
         <v>27</v>
       </c>
-      <c r="B8">
+      <c r="D8">
         <v>84000</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C9">
         <v>32</v>
       </c>
-      <c r="B9">
+      <c r="D9">
         <v>150000</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C10">
         <v>25</v>
       </c>
-      <c r="B10">
+      <c r="D10">
         <v>33000</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C11">
         <v>35</v>
       </c>
-      <c r="B11">
+      <c r="D11">
         <v>65000</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C12">
         <v>26</v>
       </c>
-      <c r="B12">
+      <c r="D12">
         <v>80000</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C13">
         <v>26</v>
       </c>
-      <c r="B13">
+      <c r="D13">
         <v>52000</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C14">
         <v>20</v>
       </c>
-      <c r="B14">
+      <c r="D14">
         <v>86000</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C15">
         <v>32</v>
       </c>
-      <c r="B15">
+      <c r="D15">
         <v>18000</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C16">
         <v>18</v>
       </c>
-      <c r="B16">
+      <c r="D16">
         <v>82000</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C17">
         <v>29</v>
       </c>
-      <c r="B17">
+      <c r="D17">
         <v>80000</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C18">
         <v>47</v>
       </c>
-      <c r="B18">
+      <c r="D18">
         <v>25000</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C19">
         <v>45</v>
       </c>
-      <c r="B19">
+      <c r="D19">
         <v>26000</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C20">
         <v>46</v>
       </c>
-      <c r="B20">
+      <c r="D20">
         <v>28000</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C21">
         <v>48</v>
       </c>
-      <c r="B21">
+      <c r="D21">
         <v>29000</v>
       </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C22">
         <v>45</v>
       </c>
-      <c r="B22">
+      <c r="D22">
         <v>22000</v>
       </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C23">
         <v>47</v>
       </c>
-      <c r="B23">
+      <c r="D23">
         <v>49000</v>
       </c>
-      <c r="C23">
+      <c r="E23">
         <v>1</v>
       </c>
     </row>

</xml_diff>